<commit_message>
Add remaining graphs and interactions with wind and solar strategy
</commit_message>
<xml_diff>
--- a/app/data/graphs_data.xlsx
+++ b/app/data/graphs_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\HES-SO\VI\Projet\SwissNuclearExit\graphs_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jermo\Documents\SwissNuclearExit\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Énergies renouvelables" sheetId="2" r:id="rId3"/>
     <sheet name="Conso ménages suisses" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -611,31 +611,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="11" t="s">
         <v>32</v>
@@ -17023,7 +17025,7 @@
       <c r="XFC1"/>
       <c r="XFD1"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="16" t="s">
         <v>22</v>
@@ -17049,7 +17051,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>16</v>
@@ -17103,7 +17105,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
@@ -17163,7 +17165,7 @@
         <v>-5491</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
@@ -17215,7 +17217,7 @@
         <v>-33885</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
@@ -17267,7 +17269,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -17319,7 +17321,7 @@
         <v>-67190</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -17371,7 +17373,7 @@
         <v>9275</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
@@ -17422,7 +17424,7 @@
         <v>2855</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
@@ -17473,7 +17475,7 @@
         <v>10197</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
@@ -17526,7 +17528,7 @@
         <v>-3406</v>
       </c>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
@@ -17578,7 +17580,7 @@
         <v>17603</v>
       </c>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
@@ -17598,16 +17600,16 @@
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -17621,7 +17623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1960</v>
       </c>
@@ -17639,7 +17641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1961</v>
       </c>
@@ -17657,7 +17659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1962</v>
       </c>
@@ -17675,7 +17677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1963</v>
       </c>
@@ -17693,7 +17695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1964</v>
       </c>
@@ -17711,7 +17713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1965</v>
       </c>
@@ -17729,7 +17731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1966</v>
       </c>
@@ -17747,7 +17749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1967</v>
       </c>
@@ -17765,7 +17767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1968</v>
       </c>
@@ -17783,7 +17785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1969</v>
       </c>
@@ -17801,7 +17803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1970</v>
       </c>
@@ -17819,7 +17821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1971</v>
       </c>
@@ -17837,7 +17839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1972</v>
       </c>
@@ -17855,7 +17857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1973</v>
       </c>
@@ -17873,7 +17875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1974</v>
       </c>
@@ -17891,7 +17893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1975</v>
       </c>
@@ -17909,7 +17911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1976</v>
       </c>
@@ -17927,7 +17929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1977</v>
       </c>
@@ -17945,7 +17947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1978</v>
       </c>
@@ -17963,7 +17965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1979</v>
       </c>
@@ -17981,7 +17983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1980</v>
       </c>
@@ -17999,7 +18001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1981</v>
       </c>
@@ -18017,7 +18019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1982</v>
       </c>
@@ -18035,7 +18037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1983</v>
       </c>
@@ -18053,7 +18055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1984</v>
       </c>
@@ -18071,7 +18073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1985</v>
       </c>
@@ -18089,7 +18091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1986</v>
       </c>
@@ -18107,7 +18109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1987</v>
       </c>
@@ -18125,7 +18127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1988</v>
       </c>
@@ -18148,7 +18150,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1989</v>
       </c>
@@ -18171,7 +18173,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1990</v>
       </c>
@@ -18194,7 +18196,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1991</v>
       </c>
@@ -18217,7 +18219,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1992</v>
       </c>
@@ -18240,7 +18242,7 @@
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1993</v>
       </c>
@@ -18263,7 +18265,7 @@
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1994</v>
       </c>
@@ -18286,7 +18288,7 @@
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1995</v>
       </c>
@@ -18309,7 +18311,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1996</v>
       </c>
@@ -18332,7 +18334,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1997</v>
       </c>
@@ -18355,7 +18357,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1998</v>
       </c>
@@ -18378,7 +18380,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1999</v>
       </c>
@@ -18401,7 +18403,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2000</v>
       </c>
@@ -18424,7 +18426,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2001</v>
       </c>
@@ -18447,7 +18449,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2002</v>
       </c>
@@ -18470,7 +18472,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2003</v>
       </c>
@@ -18493,7 +18495,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2004</v>
       </c>
@@ -18516,7 +18518,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2005</v>
       </c>
@@ -18539,7 +18541,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2006</v>
       </c>
@@ -18562,7 +18564,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2007</v>
       </c>
@@ -18585,7 +18587,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2008</v>
       </c>
@@ -18608,7 +18610,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2009</v>
       </c>
@@ -18631,7 +18633,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2010</v>
       </c>
@@ -18654,7 +18656,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2011</v>
       </c>
@@ -18675,9 +18677,11 @@
         <v>17942</v>
       </c>
       <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
+      <c r="I92" s="1">
+        <v>9458</v>
+      </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2012</v>
       </c>
@@ -18698,9 +18702,11 @@
         <v>18333</v>
       </c>
       <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
+      <c r="I93" s="1">
+        <v>7972</v>
+      </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2013</v>
       </c>
@@ -18721,9 +18727,11 @@
         <v>18768</v>
       </c>
       <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
+      <c r="I94" s="1">
+        <v>3027</v>
+      </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2014</v>
       </c>
@@ -18744,98 +18752,112 @@
         <v>18287</v>
       </c>
       <c r="H95" s="1"/>
-      <c r="I95" s="1"/>
+      <c r="I95" s="1">
+        <v>3029</v>
+      </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
+      <c r="E96" s="1">
+        <f>D95+E95</f>
+        <v>28817</v>
+      </c>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
-      <c r="I96" s="1"/>
+      <c r="I96" s="1">
+        <v>2884</v>
+      </c>
     </row>
-    <row r="116" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I97" s="1">
+        <f>SUM(I92:I96)</f>
+        <v>26370</v>
+      </c>
+    </row>
+    <row r="116" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S116" s="4"/>
       <c r="T116" s="4"/>
     </row>
-    <row r="117" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S117" s="4"/>
       <c r="T117" s="4"/>
     </row>
-    <row r="118" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S118" s="4"/>
       <c r="T118" s="4"/>
     </row>
-    <row r="119" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S119" s="4"/>
       <c r="T119" s="4"/>
     </row>
-    <row r="120" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="120" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S120" s="4"/>
       <c r="T120" s="4"/>
     </row>
-    <row r="121" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S121" s="4"/>
       <c r="T121" s="4"/>
     </row>
-    <row r="122" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S122" s="4"/>
       <c r="T122" s="4"/>
     </row>
-    <row r="123" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S123" s="4"/>
       <c r="T123" s="4"/>
     </row>
-    <row r="124" spans="19:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S124" s="4"/>
       <c r="T124" s="4"/>
     </row>
-    <row r="160" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H160" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H162" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H163" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H164" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="165" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="165" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H165" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="166" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H166" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H167" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H168" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H169" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H170" t="s">
         <v>5</v>
       </c>
@@ -18858,37 +18880,36 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.54296875" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" customWidth="1"/>
     <col min="21" max="21" width="31" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>54</v>
       </c>
@@ -18920,7 +18941,7 @@
       <c r="AA1" s="11"/>
       <c r="AB1" s="11"/>
     </row>
-    <row r="2" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="18" t="s">
@@ -18956,7 +18977,7 @@
       <c r="AA2" s="18"/>
       <c r="AB2" s="18"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -19012,7 +19033,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>55</v>
       </c>
@@ -19102,7 +19123,7 @@
         <v>-5491</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>55</v>
       </c>
@@ -19192,7 +19213,7 @@
         <v>-33885</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>55</v>
       </c>
@@ -19282,7 +19303,7 @@
         <v>43716</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
@@ -19372,7 +19393,7 @@
         <v>-67190</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>55</v>
       </c>
@@ -19462,7 +19483,7 @@
         <v>9275</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>55</v>
       </c>
@@ -19551,7 +19572,7 @@
         <v>2855</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>55</v>
       </c>
@@ -19640,7 +19661,7 @@
         <v>10197</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>55</v>
       </c>
@@ -19731,7 +19752,7 @@
         <v>-3406</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>55</v>
       </c>
@@ -19840,20 +19861,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
@@ -19861,7 +19882,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -19872,7 +19893,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -19897,13 +19918,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -19911,7 +19932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1988</v>
       </c>
@@ -19919,7 +19940,7 @@
         <v>12668</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1989</v>
       </c>
@@ -19927,7 +19948,7 @@
         <v>12875</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1990</v>
       </c>
@@ -19935,7 +19956,7 @@
         <v>13213</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1991</v>
       </c>
@@ -19943,7 +19964,7 @@
         <v>13848</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1992</v>
       </c>
@@ -19951,7 +19972,7 @@
         <v>14166</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>1993</v>
       </c>
@@ -19959,7 +19980,7 @@
         <v>14172</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1994</v>
       </c>
@@ -19967,7 +19988,7 @@
         <v>14193</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1995</v>
       </c>
@@ -19975,7 +19996,7 @@
         <v>14680</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>1996</v>
       </c>
@@ -19983,7 +20004,7 @@
         <v>15271</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>1997</v>
       </c>
@@ -19991,7 +20012,7 @@
         <v>14859</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1998</v>
       </c>
@@ -19999,7 +20020,7 @@
         <v>15122</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1999</v>
       </c>
@@ -20007,7 +20028,7 @@
         <v>15558</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2000</v>
       </c>
@@ -20015,7 +20036,7 @@
         <v>15727</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2001</v>
       </c>
@@ -20023,7 +20044,7 @@
         <v>16080</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>2002</v>
       </c>
@@ -20031,7 +20052,7 @@
         <v>16291</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>2003</v>
       </c>
@@ -20039,7 +20060,7 @@
         <v>16679</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2004</v>
       </c>
@@ -20047,7 +20068,7 @@
         <v>17114</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>2005</v>
       </c>
@@ -20055,7 +20076,7 @@
         <v>17624</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>2006</v>
       </c>
@@ -20063,7 +20084,7 @@
         <v>17702</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>2007</v>
       </c>
@@ -20071,7 +20092,7 @@
         <v>17472</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>2008</v>
       </c>
@@ -20079,7 +20100,7 @@
         <v>17897</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>2009</v>
       </c>
@@ -20087,7 +20108,7 @@
         <v>17920</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>2010</v>
       </c>
@@ -20095,7 +20116,7 @@
         <v>18618</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>2011</v>
       </c>
@@ -20103,7 +20124,7 @@
         <v>17942</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>2012</v>
       </c>
@@ -20111,7 +20132,7 @@
         <v>18333</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>2013</v>
       </c>
@@ -20119,7 +20140,7 @@
         <v>18768</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>2014</v>
       </c>

</xml_diff>